<commit_message>
V.1.1 Crocek Absen Perhari
</commit_message>
<xml_diff>
--- a/be-sistem-croscek-kehadiran/Data informasi kode jadwal.xlsx
+++ b/be-sistem-croscek-kehadiran/Data informasi kode jadwal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Magang Hub\Project\sistem-croscek-kehadiran\src\assets\data-jadwal-dan-kehadiran-karyawan-harian\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Magang Hub\Project\be-sistem-croscek-kehadiran\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4E17779-796C-4176-A51B-DCF68B0F093D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8C012C-6811-47C9-8170-30030E460D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{DCCC9DE1-FAEF-460B-B43C-21A7BCCE5728}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="153">
   <si>
     <t>No.</t>
   </si>
@@ -548,7 +548,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -564,6 +564,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFBFBFB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -795,7 +801,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -871,6 +877,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1192,15 +1210,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B83797-3A07-477A-8286-E61583CA7F7E}">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:S44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J44"/>
+      <selection activeCell="O3" sqref="O3:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -1230,7 +1248,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="25"/>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -1246,7 +1264,7 @@
       <c r="I2" s="21"/>
       <c r="J2" s="23"/>
     </row>
-    <row r="3" spans="1:10" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>11</v>
       </c>
@@ -1273,8 +1291,32 @@
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="11"/>
-    </row>
-    <row r="4" spans="1:10" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L3" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="O3" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="P3" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="30">
+        <v>0</v>
+      </c>
+      <c r="R3" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="S3" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>16</v>
       </c>
@@ -1301,8 +1343,32 @@
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="13"/>
-    </row>
-    <row r="5" spans="1:10" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L4" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="M4" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="O4" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="P4" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="30">
+        <v>0</v>
+      </c>
+      <c r="R4" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="S4" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>19</v>
       </c>
@@ -1329,8 +1395,32 @@
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="13"/>
-    </row>
-    <row r="6" spans="1:10" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L5" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="M5" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="O5" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="P5" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="30">
+        <v>0</v>
+      </c>
+      <c r="R5" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="S5" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -1357,8 +1447,32 @@
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="13"/>
-    </row>
-    <row r="7" spans="1:10" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L6" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="M6" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O6" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="P6" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="30">
+        <v>0</v>
+      </c>
+      <c r="R6" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="S6" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>25</v>
       </c>
@@ -1385,8 +1499,32 @@
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="13"/>
-    </row>
-    <row r="8" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L7" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="M7" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="O7" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="P7" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="30">
+        <v>0</v>
+      </c>
+      <c r="R7" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="S7" s="28" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>30</v>
       </c>
@@ -1414,7 +1552,7 @@
       <c r="I8" s="7"/>
       <c r="J8" s="13"/>
     </row>
-    <row r="9" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>34</v>
       </c>
@@ -1442,7 +1580,7 @@
       <c r="I9" s="7"/>
       <c r="J9" s="13"/>
     </row>
-    <row r="10" spans="1:10" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>38</v>
       </c>
@@ -1470,7 +1608,7 @@
       <c r="I10" s="7"/>
       <c r="J10" s="13"/>
     </row>
-    <row r="11" spans="1:10" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>42</v>
       </c>
@@ -1498,7 +1636,7 @@
       <c r="I11" s="7"/>
       <c r="J11" s="13"/>
     </row>
-    <row r="12" spans="1:10" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>45</v>
       </c>
@@ -1526,7 +1664,7 @@
       <c r="I12" s="7"/>
       <c r="J12" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>47</v>
       </c>
@@ -1554,7 +1692,7 @@
       <c r="I13" s="7"/>
       <c r="J13" s="13"/>
     </row>
-    <row r="14" spans="1:10" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>49</v>
       </c>
@@ -1582,57 +1720,57 @@
       <c r="I14" s="7"/>
       <c r="J14" s="13"/>
     </row>
-    <row r="15" spans="1:10" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
+    <row r="15" spans="1:19" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="B15" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="30">
         <v>0</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="30">
         <v>0</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="28" t="s">
         <v>15</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="13"/>
     </row>
-    <row r="16" spans="1:10" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
+    <row r="16" spans="1:19" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="6" t="s">
+      <c r="B16" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="30">
         <v>0</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="30">
         <v>0</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="28" t="s">
         <v>15</v>
       </c>
       <c r="I16" s="7"/>
@@ -1779,28 +1917,28 @@
       <c r="J21" s="13"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="B22" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="30">
         <v>0</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F22" s="30">
         <v>0</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="H22" s="28" t="s">
         <v>15</v>
       </c>
       <c r="I22" s="7"/>
@@ -2031,28 +2169,28 @@
       <c r="J30" s="13"/>
     </row>
     <row r="31" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="6" t="s">
+      <c r="B31" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="E31" s="8">
+      <c r="E31" s="30">
         <v>0</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F31" s="30">
         <v>0</v>
       </c>
-      <c r="G31" s="6" t="s">
+      <c r="G31" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="H31" s="6" t="s">
+      <c r="H31" s="28" t="s">
         <v>15</v>
       </c>
       <c r="I31" s="7"/>
@@ -2251,28 +2389,28 @@
       <c r="J38" s="13"/>
     </row>
     <row r="39" spans="1:10" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E39" s="30">
         <v>0</v>
       </c>
-      <c r="F39" s="8">
+      <c r="F39" s="30">
         <v>0</v>
       </c>
-      <c r="G39" s="6" t="s">
+      <c r="G39" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="H39" s="6" t="s">
+      <c r="H39" s="28" t="s">
         <v>131</v>
       </c>
       <c r="I39" s="7"/>

</xml_diff>